<commit_message>
Added more Excel functionality, added Unit test for excel classes, Added more functionality for data analysis classes
</commit_message>
<xml_diff>
--- a/EpamTask06/ExcelFiles/Летняя Сессия 2018 (ИТ-11).xlsx
+++ b/EpamTask06/ExcelFiles/Летняя Сессия 2018 (ИТ-11).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Студент</t>
   </si>
@@ -35,15 +35,24 @@
     <t>Павел Свинтицкий</t>
   </si>
   <si>
+    <t>7,5</t>
+  </si>
+  <si>
     <t>Петр Петров</t>
   </si>
   <si>
     <t>Свин Павлицкий</t>
   </si>
   <si>
+    <t>5,25</t>
+  </si>
+  <si>
     <t>Петр Иванов</t>
   </si>
   <si>
+    <t>5,5</t>
+  </si>
+  <si>
     <t>Павел Иванов</t>
   </si>
   <si>
@@ -51,6 +60,9 @@
   </si>
   <si>
     <t>Иван Иванов</t>
+  </si>
+  <si>
+    <t>7,25</t>
   </si>
   <si>
     <t>Иван Петров</t>
@@ -90,9 +102,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -375,15 +386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -397,13 +402,13 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>7.5</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -411,31 +416,31 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>5.25</v>
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5.5</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>7.5</v>
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -443,18 +448,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7.25</v>
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>7.25</v>
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>